<commit_message>
changes on corte de caja
</commit_message>
<xml_diff>
--- a/public/reportTemplates/template.xlsx
+++ b/public/reportTemplates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgeivangomez/Documents/Projects/DELFINITI/delfiniti-app/public/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEDC170-9199-5949-AB6D-0DC170DBD46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F124595-3F67-CF4A-80D0-F7353D31607A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="4720" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8600" yWindow="4100" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" style="1"/>
     <col min="5" max="5" width="24.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
   </cols>

</xml_diff>